<commit_message>
só será feita alguma alteração caso não tenha ok
</commit_message>
<xml_diff>
--- a/projetov2.xlsx
+++ b/projetov2.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -479,9 +479,6 @@
       <c r="B2" t="n">
         <v>112022</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>110,92</t>
@@ -502,10 +499,6 @@
       <c r="B3" t="n">
         <v>112022</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>ok</t>
@@ -521,14 +514,11 @@
       <c r="B4" t="n">
         <v>112022</v>
       </c>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>11066,30</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>ok</t>

</xml_diff>

<commit_message>
sem ok para testar
</commit_message>
<xml_diff>
--- a/projetov2.xlsx
+++ b/projetov2.xlsx
@@ -1,32 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <charset val="1"/>
+      <family val="0"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,21 +69,42 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -421,111 +461,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="2">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>empresa</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>dia</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>comenc</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>semenc</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>difativo</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>difauc</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>feita</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="2">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>LEIKA</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="n">
         <v>112022</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>110,92</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="2">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>PICANHA</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>112022</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="4" ht="15" customHeight="1" s="2">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>MECPEL</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>112022</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>11066,30</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>ok</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>